<commit_message>
Updated analysis for longevity of 2023. New outline for oil content + longevity paper
</commit_message>
<xml_diff>
--- a/results/2022/PCA genstat results.xlsx
+++ b/results/2022/PCA genstat results.xlsx
@@ -199,14 +199,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,7 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25BB1C9-BBEC-4E8A-95B3-1E4B20DC9702}">
   <dimension ref="A2:T44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -708,7 +707,7 @@
       <c r="M2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" t="s">
         <v>17</v>
       </c>
       <c r="O2" t="s">
@@ -2231,31 +2230,31 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="H35" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I35" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="J35" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2263,31 +2262,31 @@
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="4">
-        <v>1</v>
-      </c>
-      <c r="C36" s="4">
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3">
         <v>-0.57596499999999995</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="3">
         <v>1.562437E-2</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <v>0.16221964999999999</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="3">
         <v>-7.0016229999999999E-2</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="3">
         <v>0.20544852999999999</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="3">
         <v>-0.19872745</v>
       </c>
-      <c r="I36" s="4">
+      <c r="I36" s="3">
         <v>-0.20686260000000001</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36" s="3">
         <v>0.17354892999999999</v>
       </c>
     </row>
@@ -2295,31 +2294,31 @@
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <v>-0.57596497000000002</v>
       </c>
-      <c r="C37" s="4">
-        <v>1</v>
-      </c>
-      <c r="D37" s="4">
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3">
         <v>0.56065675000000004</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="3">
         <v>-6.4124799999999996E-2</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="3">
         <v>0.19383316</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="3">
         <v>-0.24077107</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="3">
         <v>0.27213797000000001</v>
       </c>
-      <c r="I37" s="4">
+      <c r="I37" s="3">
         <v>0.21913182</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37" s="3">
         <v>-0.53854760000000002</v>
       </c>
     </row>
@@ -2327,31 +2326,31 @@
       <c r="A38" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="3">
         <v>1.562437E-2</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="3">
         <v>0.56065679999999996</v>
       </c>
-      <c r="D38" s="4">
-        <v>1</v>
-      </c>
-      <c r="E38" s="4">
+      <c r="D38" s="3">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3">
         <v>-3.942433E-2</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="3">
         <v>7.3537640000000001E-2</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="3">
         <v>-0.1709434</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="3">
         <v>0.19625253000000001</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38" s="3">
         <v>5.531026E-2</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38" s="3">
         <v>-0.62322345999999995</v>
       </c>
     </row>
@@ -2359,31 +2358,31 @@
       <c r="A39" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="3">
         <v>0.16221964999999999</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="3">
         <v>-6.4124799999999996E-2</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="3">
         <v>-3.942433E-2</v>
       </c>
-      <c r="E39" s="4">
-        <v>1</v>
-      </c>
-      <c r="F39" s="4">
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3">
         <v>-0.36130190000000001</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="3">
         <v>0.55444775999999996</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39" s="3">
         <v>-0.40183848</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39" s="3">
         <v>-5.9482100000000003E-2</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J39" s="3">
         <v>-5.0096809999999999E-2</v>
       </c>
     </row>
@@ -2391,31 +2390,31 @@
       <c r="A40" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="3">
         <v>-7.0016229999999999E-2</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="3">
         <v>0.19383320000000001</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="3">
         <v>7.3537640000000001E-2</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="3">
         <v>-0.36130190000000001</v>
       </c>
-      <c r="F40" s="4">
-        <v>1</v>
-      </c>
-      <c r="G40" s="4">
+      <c r="F40" s="3">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3">
         <v>-0.81552986999999999</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40" s="3">
         <v>0.79973958999999994</v>
       </c>
-      <c r="I40" s="4">
+      <c r="I40" s="3">
         <v>-5.8633900000000003E-2</v>
       </c>
-      <c r="J40" s="4">
+      <c r="J40" s="3">
         <v>-0.27436703000000001</v>
       </c>
     </row>
@@ -2423,31 +2422,31 @@
       <c r="A41" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="3">
         <v>0.20544852999999999</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="3">
         <v>-0.24077109999999999</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="3">
         <v>-0.1709434</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="3">
         <v>0.55444775999999996</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F41" s="3">
         <v>-0.81552986999999999</v>
       </c>
-      <c r="G41" s="4">
-        <v>1</v>
-      </c>
-      <c r="H41" s="4">
+      <c r="G41" s="3">
+        <v>1</v>
+      </c>
+      <c r="H41" s="3">
         <v>-0.90873404999999996</v>
       </c>
-      <c r="I41" s="4">
+      <c r="I41" s="3">
         <v>3.990556E-2</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J41" s="3">
         <v>0.21208115</v>
       </c>
     </row>
@@ -2455,31 +2454,31 @@
       <c r="A42" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="3">
         <v>-0.19872745</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="3">
         <v>0.27213799999999999</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="3">
         <v>0.19625253000000001</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="3">
         <v>-0.40183848</v>
       </c>
-      <c r="F42" s="4">
+      <c r="F42" s="3">
         <v>0.79973958999999994</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="3">
         <v>-0.90873404999999996</v>
       </c>
-      <c r="H42" s="4">
-        <v>1</v>
-      </c>
-      <c r="I42" s="4">
+      <c r="H42" s="3">
+        <v>1</v>
+      </c>
+      <c r="I42" s="3">
         <v>5.6789729999999997E-2</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="3">
         <v>-0.26741181000000003</v>
       </c>
     </row>
@@ -2487,31 +2486,31 @@
       <c r="A43" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="3">
         <v>-0.20686260000000001</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="3">
         <v>0.21913179999999999</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D43" s="3">
         <v>5.531026E-2</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="3">
         <v>-5.9482100000000003E-2</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F43" s="3">
         <v>-5.8633900000000003E-2</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="3">
         <v>3.990556E-2</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H43" s="3">
         <v>5.6789729999999997E-2</v>
       </c>
-      <c r="I43" s="4">
-        <v>1</v>
-      </c>
-      <c r="J43" s="4">
+      <c r="I43" s="3">
+        <v>1</v>
+      </c>
+      <c r="J43" s="3">
         <v>-0.39321337000000001</v>
       </c>
     </row>
@@ -2519,47 +2518,35 @@
       <c r="A44" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="3">
         <v>0.17354892999999999</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="3">
         <v>-0.53854760000000002</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="3">
         <v>-0.62322345999999995</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="3">
         <v>-5.0096809999999999E-2</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F44" s="3">
         <v>-0.27436703000000001</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44" s="3">
         <v>0.21208115</v>
       </c>
-      <c r="H44" s="4">
+      <c r="H44" s="3">
         <v>-0.26741181000000003</v>
       </c>
-      <c r="I44" s="4">
+      <c r="I44" s="3">
         <v>-0.39321337000000001</v>
       </c>
-      <c r="J44" s="4">
+      <c r="J44" s="3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:T21">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B25:F33">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -2582,6 +2569,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B3:T21">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>